<commit_message>
eva initially working, a lot of mismatched data?
</commit_message>
<xml_diff>
--- a/data/eva_jc_blank.xlsx
+++ b/data/eva_jc_blank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://windlecc-my.sharepoint.com/personal/sung_windlecc_com/Documents/QuickBooks Related/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{530E1431-2F57-42C6-A83F-5B9834A58650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDA422C2-9E10-4249-A639-69B72B7F0E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="450" yWindow="1020" windowWidth="15930" windowHeight="14100" xr2:uid="{E28F7204-FE0D-451C-ABE2-A8D89BD26980}"/>
   </bookViews>
@@ -581,13 +581,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E51" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="3" width="3" style="3" customWidth="1"/>
     <col min="4" max="4" width="38" style="16" customWidth="1"/>

</xml_diff>

<commit_message>
attempting to fix draw line, misc formatting
</commit_message>
<xml_diff>
--- a/data/eva_jc_blank.xlsx
+++ b/data/eva_jc_blank.xlsx
@@ -521,7 +521,7 @@
       <c r="Y5" s="20"/>
       <c r="Z5" s="20"/>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
@@ -532,7 +532,7 @@
       <c r="H6" s="24"/>
       <c r="I6" s="11"/>
     </row>
-    <row r="7">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="22"/>
@@ -543,7 +543,7 @@
       <c r="H7" s="24"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="22"/>
@@ -554,7 +554,7 @@
       <c r="H8" s="24"/>
       <c r="I8" s="11"/>
     </row>
-    <row r="9">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="22"/>
@@ -565,7 +565,7 @@
       <c r="H9" s="24"/>
       <c r="I9" s="11"/>
     </row>
-    <row r="10">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="22"/>
@@ -576,7 +576,7 @@
       <c r="H10" s="24"/>
       <c r="I10" s="11"/>
     </row>
-    <row r="11">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="22"/>
@@ -587,7 +587,7 @@
       <c r="H11" s="24"/>
       <c r="I11" s="11"/>
     </row>
-    <row r="12">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="21"/>
       <c r="B12" s="21"/>
       <c r="C12" s="22"/>
@@ -598,7 +598,7 @@
       <c r="H12" s="24"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="13">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22"/>
@@ -609,7 +609,7 @@
       <c r="H13" s="24"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
@@ -620,7 +620,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="11"/>
     </row>
-    <row r="15">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22"/>
@@ -631,7 +631,7 @@
       <c r="H15" s="24"/>
       <c r="I15" s="11"/>
     </row>
-    <row r="16">
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="22"/>
@@ -642,7 +642,7 @@
       <c r="H16" s="24"/>
       <c r="I16" s="11"/>
     </row>
-    <row r="17">
+    <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="22"/>
@@ -653,7 +653,7 @@
       <c r="H17" s="24"/>
       <c r="I17" s="11"/>
     </row>
-    <row r="18">
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
       <c r="C18" s="22"/>
@@ -664,7 +664,7 @@
       <c r="H18" s="24"/>
       <c r="I18" s="11"/>
     </row>
-    <row r="19">
+    <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
@@ -675,7 +675,7 @@
       <c r="H19" s="24"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20">
+    <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
       <c r="C20" s="22"/>
@@ -11191,281 +11191,6 @@
       <c r="H975" s="24"/>
       <c r="I975" s="11"/>
     </row>
-    <row r="976" ht="15.75" customHeight="1">
-      <c r="A976" s="21"/>
-      <c r="B976" s="21"/>
-      <c r="C976" s="22"/>
-      <c r="D976" s="23"/>
-      <c r="E976" s="4"/>
-      <c r="F976" s="24"/>
-      <c r="G976" s="4"/>
-      <c r="H976" s="24"/>
-      <c r="I976" s="11"/>
-    </row>
-    <row r="977" ht="15.75" customHeight="1">
-      <c r="A977" s="21"/>
-      <c r="B977" s="21"/>
-      <c r="C977" s="22"/>
-      <c r="D977" s="23"/>
-      <c r="E977" s="4"/>
-      <c r="F977" s="24"/>
-      <c r="G977" s="4"/>
-      <c r="H977" s="24"/>
-      <c r="I977" s="11"/>
-    </row>
-    <row r="978" ht="15.75" customHeight="1">
-      <c r="A978" s="21"/>
-      <c r="B978" s="21"/>
-      <c r="C978" s="22"/>
-      <c r="D978" s="23"/>
-      <c r="E978" s="4"/>
-      <c r="F978" s="24"/>
-      <c r="G978" s="4"/>
-      <c r="H978" s="24"/>
-      <c r="I978" s="11"/>
-    </row>
-    <row r="979" ht="15.75" customHeight="1">
-      <c r="A979" s="21"/>
-      <c r="B979" s="21"/>
-      <c r="C979" s="22"/>
-      <c r="D979" s="23"/>
-      <c r="E979" s="4"/>
-      <c r="F979" s="24"/>
-      <c r="G979" s="4"/>
-      <c r="H979" s="24"/>
-      <c r="I979" s="11"/>
-    </row>
-    <row r="980" ht="15.75" customHeight="1">
-      <c r="A980" s="21"/>
-      <c r="B980" s="21"/>
-      <c r="C980" s="22"/>
-      <c r="D980" s="23"/>
-      <c r="E980" s="4"/>
-      <c r="F980" s="24"/>
-      <c r="G980" s="4"/>
-      <c r="H980" s="24"/>
-      <c r="I980" s="11"/>
-    </row>
-    <row r="981" ht="15.75" customHeight="1">
-      <c r="A981" s="21"/>
-      <c r="B981" s="21"/>
-      <c r="C981" s="22"/>
-      <c r="D981" s="23"/>
-      <c r="E981" s="4"/>
-      <c r="F981" s="24"/>
-      <c r="G981" s="4"/>
-      <c r="H981" s="24"/>
-      <c r="I981" s="11"/>
-    </row>
-    <row r="982" ht="15.75" customHeight="1">
-      <c r="A982" s="21"/>
-      <c r="B982" s="21"/>
-      <c r="C982" s="22"/>
-      <c r="D982" s="23"/>
-      <c r="E982" s="4"/>
-      <c r="F982" s="24"/>
-      <c r="G982" s="4"/>
-      <c r="H982" s="24"/>
-      <c r="I982" s="11"/>
-    </row>
-    <row r="983" ht="15.75" customHeight="1">
-      <c r="A983" s="21"/>
-      <c r="B983" s="21"/>
-      <c r="C983" s="22"/>
-      <c r="D983" s="23"/>
-      <c r="E983" s="4"/>
-      <c r="F983" s="24"/>
-      <c r="G983" s="4"/>
-      <c r="H983" s="24"/>
-      <c r="I983" s="11"/>
-    </row>
-    <row r="984" ht="15.75" customHeight="1">
-      <c r="A984" s="21"/>
-      <c r="B984" s="21"/>
-      <c r="C984" s="22"/>
-      <c r="D984" s="23"/>
-      <c r="E984" s="4"/>
-      <c r="F984" s="24"/>
-      <c r="G984" s="4"/>
-      <c r="H984" s="24"/>
-      <c r="I984" s="11"/>
-    </row>
-    <row r="985" ht="15.75" customHeight="1">
-      <c r="A985" s="21"/>
-      <c r="B985" s="21"/>
-      <c r="C985" s="22"/>
-      <c r="D985" s="23"/>
-      <c r="E985" s="4"/>
-      <c r="F985" s="24"/>
-      <c r="G985" s="4"/>
-      <c r="H985" s="24"/>
-      <c r="I985" s="11"/>
-    </row>
-    <row r="986" ht="15.75" customHeight="1">
-      <c r="A986" s="21"/>
-      <c r="B986" s="21"/>
-      <c r="C986" s="22"/>
-      <c r="D986" s="23"/>
-      <c r="E986" s="4"/>
-      <c r="F986" s="24"/>
-      <c r="G986" s="4"/>
-      <c r="H986" s="24"/>
-      <c r="I986" s="11"/>
-    </row>
-    <row r="987" ht="15.75" customHeight="1">
-      <c r="A987" s="21"/>
-      <c r="B987" s="21"/>
-      <c r="C987" s="22"/>
-      <c r="D987" s="23"/>
-      <c r="E987" s="4"/>
-      <c r="F987" s="24"/>
-      <c r="G987" s="4"/>
-      <c r="H987" s="24"/>
-      <c r="I987" s="11"/>
-    </row>
-    <row r="988" ht="15.75" customHeight="1">
-      <c r="A988" s="21"/>
-      <c r="B988" s="21"/>
-      <c r="C988" s="22"/>
-      <c r="D988" s="23"/>
-      <c r="E988" s="4"/>
-      <c r="F988" s="24"/>
-      <c r="G988" s="4"/>
-      <c r="H988" s="24"/>
-      <c r="I988" s="11"/>
-    </row>
-    <row r="989" ht="15.75" customHeight="1">
-      <c r="A989" s="21"/>
-      <c r="B989" s="21"/>
-      <c r="C989" s="22"/>
-      <c r="D989" s="23"/>
-      <c r="E989" s="4"/>
-      <c r="F989" s="24"/>
-      <c r="G989" s="4"/>
-      <c r="H989" s="24"/>
-      <c r="I989" s="11"/>
-    </row>
-    <row r="990" ht="15.75" customHeight="1">
-      <c r="A990" s="21"/>
-      <c r="B990" s="21"/>
-      <c r="C990" s="22"/>
-      <c r="D990" s="23"/>
-      <c r="E990" s="4"/>
-      <c r="F990" s="24"/>
-      <c r="G990" s="4"/>
-      <c r="H990" s="24"/>
-      <c r="I990" s="11"/>
-    </row>
-    <row r="991" ht="15.75" customHeight="1">
-      <c r="A991" s="21"/>
-      <c r="B991" s="21"/>
-      <c r="C991" s="22"/>
-      <c r="D991" s="23"/>
-      <c r="E991" s="4"/>
-      <c r="F991" s="24"/>
-      <c r="G991" s="4"/>
-      <c r="H991" s="24"/>
-      <c r="I991" s="11"/>
-    </row>
-    <row r="992" ht="15.75" customHeight="1">
-      <c r="A992" s="21"/>
-      <c r="B992" s="21"/>
-      <c r="C992" s="22"/>
-      <c r="D992" s="23"/>
-      <c r="E992" s="4"/>
-      <c r="F992" s="24"/>
-      <c r="G992" s="4"/>
-      <c r="H992" s="24"/>
-      <c r="I992" s="11"/>
-    </row>
-    <row r="993" ht="15.75" customHeight="1">
-      <c r="A993" s="21"/>
-      <c r="B993" s="21"/>
-      <c r="C993" s="22"/>
-      <c r="D993" s="23"/>
-      <c r="E993" s="4"/>
-      <c r="F993" s="24"/>
-      <c r="G993" s="4"/>
-      <c r="H993" s="24"/>
-      <c r="I993" s="11"/>
-    </row>
-    <row r="994" ht="15.75" customHeight="1">
-      <c r="A994" s="21"/>
-      <c r="B994" s="21"/>
-      <c r="C994" s="22"/>
-      <c r="D994" s="23"/>
-      <c r="E994" s="4"/>
-      <c r="F994" s="24"/>
-      <c r="G994" s="4"/>
-      <c r="H994" s="24"/>
-      <c r="I994" s="11"/>
-    </row>
-    <row r="995" ht="15.75" customHeight="1">
-      <c r="A995" s="21"/>
-      <c r="B995" s="21"/>
-      <c r="C995" s="22"/>
-      <c r="D995" s="23"/>
-      <c r="E995" s="4"/>
-      <c r="F995" s="24"/>
-      <c r="G995" s="4"/>
-      <c r="H995" s="24"/>
-      <c r="I995" s="11"/>
-    </row>
-    <row r="996" ht="15.75" customHeight="1">
-      <c r="A996" s="21"/>
-      <c r="B996" s="21"/>
-      <c r="C996" s="22"/>
-      <c r="D996" s="23"/>
-      <c r="E996" s="4"/>
-      <c r="F996" s="24"/>
-      <c r="G996" s="4"/>
-      <c r="H996" s="24"/>
-      <c r="I996" s="11"/>
-    </row>
-    <row r="997" ht="15.75" customHeight="1">
-      <c r="A997" s="21"/>
-      <c r="B997" s="21"/>
-      <c r="C997" s="22"/>
-      <c r="D997" s="23"/>
-      <c r="E997" s="4"/>
-      <c r="F997" s="24"/>
-      <c r="G997" s="4"/>
-      <c r="H997" s="24"/>
-      <c r="I997" s="11"/>
-    </row>
-    <row r="998" ht="15.75" customHeight="1">
-      <c r="A998" s="21"/>
-      <c r="B998" s="21"/>
-      <c r="C998" s="22"/>
-      <c r="D998" s="23"/>
-      <c r="E998" s="4"/>
-      <c r="F998" s="24"/>
-      <c r="G998" s="4"/>
-      <c r="H998" s="24"/>
-      <c r="I998" s="11"/>
-    </row>
-    <row r="999" ht="15.75" customHeight="1">
-      <c r="A999" s="21"/>
-      <c r="B999" s="21"/>
-      <c r="C999" s="22"/>
-      <c r="D999" s="23"/>
-      <c r="E999" s="4"/>
-      <c r="F999" s="24"/>
-      <c r="G999" s="4"/>
-      <c r="H999" s="24"/>
-      <c r="I999" s="11"/>
-    </row>
-    <row r="1000" ht="15.75" customHeight="1">
-      <c r="A1000" s="21"/>
-      <c r="B1000" s="21"/>
-      <c r="C1000" s="22"/>
-      <c r="D1000" s="23"/>
-      <c r="E1000" s="4"/>
-      <c r="F1000" s="24"/>
-      <c r="G1000" s="4"/>
-      <c r="H1000" s="24"/>
-      <c r="I1000" s="11"/>
-    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>